<commit_message>
aggiunto esercizio in coda alla beta binomiale
</commit_message>
<xml_diff>
--- a/syllabus-and-improv/sequenzaLezioniBDA.xlsx
+++ b/syllabus-and-improv/sequenzaLezioniBDA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgio/switchdrive/teaching/BayesianProg/bda/syllabus-and-improv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2DC711-3BA8-4A42-8BBD-6B1626D7EAC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AC8023-B8F6-CB4D-A5F4-E5547EE1DA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="98">
   <si>
     <t>lezione</t>
   </si>
@@ -375,6 +375,9 @@
   </si>
   <si>
     <t>finire beta-bin; 3.9, 3.10, exe 3.11 (updating) and 3.12</t>
+  </si>
+  <si>
+    <t>normal normal, exe 5.9 e 5.10</t>
   </si>
 </sst>
 </file>
@@ -958,7 +961,7 @@
   <dimension ref="A1:X122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="175" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1058,6 +1061,9 @@
       <c r="B11" s="23">
         <f>B10+3</f>
         <v>44840</v>
+      </c>
+      <c r="C11" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fixed typos in beta-binomial and normal-normal
</commit_message>
<xml_diff>
--- a/syllabus-and-improv/sequenzaLezioniBDA.xlsx
+++ b/syllabus-and-improv/sequenzaLezioniBDA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgio/switchdrive/teaching/BayesianProg/bda/syllabus-and-improv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AC8023-B8F6-CB4D-A5F4-E5547EE1DA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6804F582-FD30-CB47-851C-97B9CBB4135C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="32000" windowHeight="16020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="101">
   <si>
     <t>lezione</t>
   </si>
@@ -374,10 +374,19 @@
     <t>exe</t>
   </si>
   <si>
-    <t>finire beta-bin; 3.9, 3.10, exe 3.11 (updating) and 3.12</t>
-  </si>
-  <si>
-    <t>normal normal, exe 5.9 e 5.10</t>
+    <t>ripresa beta; binomial likelihood; up to slide 54 (sensitivity to the prior)</t>
+  </si>
+  <si>
+    <t>finire beta-bin; 3.9, 3.10, normal-normal</t>
+  </si>
+  <si>
+    <t>MF</t>
+  </si>
+  <si>
+    <t>normal normal; 5.9, 5.10; prior su varianza</t>
+  </si>
+  <si>
+    <t>reporting analysis; normal normal (esercizio likelihood)</t>
   </si>
 </sst>
 </file>
@@ -1074,6 +1083,9 @@
         <f>B10+7</f>
         <v>44844</v>
       </c>
+      <c r="C12" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="24">
@@ -1083,7 +1095,9 @@
         <f>B12+3</f>
         <v>44847</v>
       </c>
-      <c r="C13" s="24"/>
+      <c r="C13" s="24" t="s">
+        <v>98</v>
+      </c>
       <c r="D13" s="24"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1093,6 +1107,9 @@
       <c r="B14" s="23">
         <f>B12+7</f>
         <v>44851</v>
+      </c>
+      <c r="C14" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>